<commit_message>
OW-650 fixed the failing unit tests
</commit_message>
<xml_diff>
--- a/src/test/resources/portfolio/OneIRS.xlsx
+++ b/src/test/resources/portfolio/OneIRS.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IRS-Cleared" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="FRA-Cleared" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="OIS-Cleared" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="IRS-Bilateral" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="FXSwap-Bilateral" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,8 +23,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Negative amount indicates short(sold) position
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Negative amount indicates short(sold) position
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="112">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -193,37 +234,64 @@
     <t xml:space="preserve">MaturityTrench</t>
   </si>
   <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRA_PAYMENT_DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRA_FIXING_DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counterpart Firm ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXEDLEG_PAYATSTART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLOATLEG_PAYATSTART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DiscountMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCM Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counterpart ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agreement ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEG1_VARIABLECURRENCY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEG2_VARIABLECURRENCY</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACUOSG8745</t>
   </si>
   <si>
     <t xml:space="preserve">720400TGFLH2QZV80T</t>
   </si>
   <si>
-    <t xml:space="preserve">455123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUD</t>
+    <t xml:space="preserve">455642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXN</t>
   </si>
   <si>
     <t xml:space="preserve">12:00:00.000</t>
   </si>
   <si>
-    <t xml:space="preserve">CLEARED</t>
+    <t xml:space="preserve">Bilateral</t>
   </si>
   <si>
     <t xml:space="preserve">-631,053.94</t>
   </si>
   <si>
-    <t xml:space="preserve">-621,377.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-9,676.76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42.56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CME</t>
+    <t xml:space="preserve">MARKIT_WIRE</t>
   </si>
   <si>
     <t xml:space="preserve">FIXED</t>
@@ -235,7 +303,7 @@
     <t xml:space="preserve">ModifiedFollowing</t>
   </si>
   <si>
-    <t xml:space="preserve">AUSY</t>
+    <t xml:space="preserve">MEXICO</t>
   </si>
   <si>
     <t xml:space="preserve">Act/365F</t>
@@ -244,13 +312,16 @@
     <t xml:space="preserve">10,000,000.00</t>
   </si>
   <si>
-    <t xml:space="preserve">1.25</t>
+    <t xml:space="preserve">0.08</t>
   </si>
   <si>
     <t xml:space="preserve">FLOAT</t>
   </si>
   <si>
-    <t xml:space="preserve">AUD-BBR-BBSW</t>
+    <t xml:space="preserve">28D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXN-TIIE-Banxico</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
@@ -259,82 +330,76 @@
     <t xml:space="preserve">P</t>
   </si>
   <si>
-    <t xml:space="preserve">LCH Clearnet Ltd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">549300MHCFARP0SMZV21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goldman Sachs &amp; Co.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRA_PAYMENT_DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRA_FIXING_DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counterpart Firm ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FCM Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counterpart ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agreement ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACUOUS6924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104399UHGKI1RAW91U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">455820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SGD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bilateral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,859.90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARKIT_WIRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SGSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SGD-SOR-Reuters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5513008I8OABDX7R9S44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Singapore</t>
+    <t xml:space="preserve">222105IP581HO777LM30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value_Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position_Account_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trade_Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trade_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firm_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency2_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position_leg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maturity_Date_leg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settle_Date_leg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate_leg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position_leg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maturity_Date_leg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settle_Date_leg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate_leg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpotSource_leg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpotSource_leg2</t>
   </si>
 </sst>
 </file>
@@ -346,7 +411,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY/MM/DD"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -367,6 +432,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -411,7 +483,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,10 +497,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,65 +517,64 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BE2"/>
+  <dimension ref="A1:BD1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="35.7704081632653"/>
     <col collapsed="false" hidden="false" max="49" min="49" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="52" min="50" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="51" min="50" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="6.61224489795918"/>
     <col collapsed="false" hidden="false" max="56" min="56" style="0" width="13.3622448979592"/>
     <col collapsed="false" hidden="false" max="1025" min="57" style="0" width="11.3418367346939"/>
   </cols>
@@ -531,7 +598,7 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
@@ -681,168 +748,6 @@
       <c r="BD1" s="0" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>41631</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>40882</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>43439</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>41605</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>999</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="3" t="n">
-        <v>40882</v>
-      </c>
-      <c r="AA2" s="3" t="n">
-        <v>43439</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM2" s="3" t="n">
-        <v>40882</v>
-      </c>
-      <c r="AN2" s="3" t="n">
-        <v>43439</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="AS2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AX2" s="0" t="n">
-        <v>-631053.94</v>
-      </c>
-      <c r="AY2" s="0" t="n">
-        <v>-621377.18</v>
-      </c>
-      <c r="AZ2" s="0" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="BA2" s="0" t="n">
-        <f aca="false">0.04*AZ2</f>
-        <v>400000</v>
-      </c>
-      <c r="BB2" s="0" t="n">
-        <f aca="false">175+0.0075*BA2</f>
-        <v>3175</v>
-      </c>
-      <c r="BC2" s="0" t="n">
-        <f aca="false">(3+4*BD2)/100000*AZ2</f>
-        <v>2460</v>
-      </c>
-      <c r="BD2" s="0" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="BE2" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -860,56 +765,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="39" min="37" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>10</v>
@@ -998,13 +903,13 @@
         <v>28</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="AF1" s="0" t="s">
         <v>44</v>
@@ -1041,6 +946,15 @@
       </c>
       <c r="AQ1" s="0" t="s">
         <v>55</v>
+      </c>
+      <c r="AR1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS1" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT1" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1061,66 +975,63 @@
   </sheetPr>
   <dimension ref="A1:BE1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.26530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="5.39795918367347"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="53" min="51" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="52" min="51" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="13.3622448979592"/>
     <col collapsed="false" hidden="false" max="1025" min="58" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
@@ -1258,7 +1169,7 @@
         <v>43</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="AT1" s="0" t="s">
         <v>44</v>
@@ -1315,56 +1226,53 @@
   </sheetPr>
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.3826530612245"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.5714285714286"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.3826530612245"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="19.5714285714286"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="41" min="40" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="26.7295918367347"/>
     <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
@@ -1387,125 +1295,125 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,127 +1421,127 @@
         <v>41631</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>41686</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>45338</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="3" t="n">
+        <v>41686</v>
+      </c>
+      <c r="W2" s="3" t="n">
+        <v>45338</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI2" s="3" t="n">
+        <v>41686</v>
+      </c>
+      <c r="AJ2" s="3" t="n">
+        <v>45338</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ2" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="AR2" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="AS2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>41607</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>44166</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>41605</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>999</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="W2" s="3" t="n">
-        <v>41607</v>
-      </c>
-      <c r="X2" s="3" t="n">
-        <v>44166</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ2" s="3" t="n">
-        <v>41607</v>
-      </c>
-      <c r="AK2" s="3" t="n">
-        <v>44166</v>
-      </c>
-      <c r="AL2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP2" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="AQ2" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR2" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS2" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="AT2" s="0" t="n">
-        <v>10000000</v>
+      <c r="AT2" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1645,4 +1553,145 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AB1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>